<commit_message>
ML parameters update 2022-08-29
</commit_message>
<xml_diff>
--- a/multi_stocks_multi_predictions_learning_parameters.xlsx
+++ b/multi_stocks_multi_predictions_learning_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dickli/Documents/GitHub/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B7E316-5FA0-B14A-B52B-934ABB20310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22091DA-985A-CF41-9E67-588879F8C7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1880" windowWidth="27640" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="3140" windowWidth="27640" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multi_stocks_multi_predictions_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -942,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,37 +1002,37 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>365</v>
       </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>800</v>
-      </c>
-      <c r="G2" s="4">
-        <v>50</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="E2">
+        <v>128</v>
+      </c>
+      <c r="F2">
+        <v>600</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
         <v>150</v>
       </c>
-      <c r="I2" s="4">
-        <v>100</v>
-      </c>
-      <c r="J2" s="4">
-        <v>50</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.2</v>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
       </c>
       <c r="L2" s="2">
         <v>0.8</v>
@@ -1046,37 +1046,37 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>365</v>
       </c>
-      <c r="E3" s="2">
-        <v>128</v>
-      </c>
-      <c r="F3" s="2">
-        <v>400</v>
-      </c>
-      <c r="G3" s="2">
-        <v>50</v>
-      </c>
-      <c r="H3" s="2">
-        <v>150</v>
-      </c>
-      <c r="I3" s="2">
-        <v>100</v>
-      </c>
-      <c r="J3" s="2">
-        <v>50</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0.1</v>
+      <c r="E3">
+        <v>512</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
       </c>
       <c r="L3" s="2">
         <v>0.8</v>
@@ -1090,37 +1090,37 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>365</v>
-      </c>
-      <c r="E4" s="4">
-        <v>128</v>
-      </c>
-      <c r="F4" s="4">
-        <v>600</v>
-      </c>
-      <c r="G4" s="4">
-        <v>50</v>
-      </c>
-      <c r="H4" s="4">
-        <v>150</v>
-      </c>
-      <c r="I4" s="4">
-        <v>100</v>
-      </c>
-      <c r="J4" s="4">
-        <v>50</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.1</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>730</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>250</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
       </c>
       <c r="L4" s="2">
         <v>0.8</v>
@@ -1134,36 +1134,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>365</v>
-      </c>
-      <c r="E5" s="2">
-        <v>512</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>730</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
         <v>1000</v>
       </c>
-      <c r="G5" s="2">
-        <v>50</v>
-      </c>
-      <c r="H5" s="2">
-        <v>200</v>
-      </c>
-      <c r="I5" s="2">
-        <v>100</v>
-      </c>
-      <c r="J5" s="2">
-        <v>50</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>250</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
         <v>0.2</v>
       </c>
       <c r="L5" s="2">
@@ -1178,37 +1178,37 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>365</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6">
+        <v>128</v>
+      </c>
+      <c r="F6">
         <v>600</v>
       </c>
-      <c r="G6" s="4">
-        <v>50</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
         <v>150</v>
       </c>
-      <c r="I6" s="4">
-        <v>100</v>
-      </c>
-      <c r="J6" s="4">
-        <v>50</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.2</v>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>0.1</v>
       </c>
       <c r="L6" s="2">
         <v>0.8</v>
@@ -1222,37 +1222,37 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>365</v>
       </c>
-      <c r="E7" s="4">
-        <v>128</v>
-      </c>
-      <c r="F7" s="4">
-        <v>600</v>
-      </c>
-      <c r="G7" s="4">
-        <v>50</v>
-      </c>
-      <c r="H7" s="4">
-        <v>150</v>
-      </c>
-      <c r="I7" s="4">
-        <v>100</v>
-      </c>
-      <c r="J7" s="4">
-        <v>50</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0.1</v>
+      <c r="E7">
+        <v>512</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>50</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
       </c>
       <c r="L7" s="2">
         <v>0.8</v>
@@ -1266,36 +1266,36 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>730</v>
       </c>
-      <c r="E8" s="2">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
         <v>1000</v>
       </c>
-      <c r="G8" s="2">
-        <v>40</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
         <v>250</v>
       </c>
-      <c r="I8" s="2">
-        <v>100</v>
-      </c>
-      <c r="J8" s="2">
-        <v>50</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
         <v>0.2</v>
       </c>
       <c r="L8" s="2">
@@ -1310,36 +1310,36 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>365</v>
-      </c>
-      <c r="E9" s="2">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2">
-        <v>600</v>
-      </c>
-      <c r="G9" s="2">
-        <v>50</v>
-      </c>
-      <c r="H9" s="2">
-        <v>150</v>
-      </c>
-      <c r="I9" s="2">
-        <v>100</v>
-      </c>
-      <c r="J9" s="2">
-        <v>50</v>
-      </c>
-      <c r="K9" s="2">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>730</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>250</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
         <v>0.2</v>
       </c>
       <c r="L9" s="2">
@@ -1354,37 +1354,37 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>365</v>
       </c>
-      <c r="E10" s="2">
-        <v>512</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G10" s="2">
-        <v>50</v>
-      </c>
-      <c r="H10" s="2">
-        <v>200</v>
-      </c>
-      <c r="I10" s="2">
-        <v>100</v>
-      </c>
-      <c r="J10" s="2">
-        <v>50</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.2</v>
+      <c r="E10">
+        <v>128</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>150</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <v>0.1</v>
       </c>
       <c r="L10" s="2">
         <v>0.8</v>
@@ -1398,36 +1398,36 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>365</v>
       </c>
-      <c r="E11" s="2">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2">
-        <v>600</v>
-      </c>
-      <c r="G11" s="2">
-        <v>50</v>
-      </c>
-      <c r="H11" s="2">
-        <v>150</v>
-      </c>
-      <c r="I11" s="2">
-        <v>100</v>
-      </c>
-      <c r="J11" s="2">
-        <v>50</v>
-      </c>
-      <c r="K11" s="2">
+      <c r="E11">
+        <v>512</v>
+      </c>
+      <c r="F11">
+        <v>1000</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
         <v>0.2</v>
       </c>
       <c r="L11" s="2">
@@ -1442,36 +1442,36 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>365</v>
-      </c>
-      <c r="E12" s="3">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3">
-        <v>600</v>
-      </c>
-      <c r="G12" s="3">
-        <v>50</v>
-      </c>
-      <c r="H12" s="3">
-        <v>150</v>
-      </c>
-      <c r="I12" s="3">
-        <v>100</v>
-      </c>
-      <c r="J12" s="3">
-        <v>50</v>
-      </c>
-      <c r="K12" s="3">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>730</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1000</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>250</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>50</v>
+      </c>
+      <c r="K12">
         <v>0.2</v>
       </c>
       <c r="L12" s="2">
@@ -1486,36 +1486,36 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>730</v>
       </c>
-      <c r="E13" s="3">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
         <v>1000</v>
       </c>
-      <c r="G13" s="3">
-        <v>50</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13">
+        <v>40</v>
+      </c>
+      <c r="H13">
         <v>250</v>
       </c>
-      <c r="I13" s="3">
-        <v>100</v>
-      </c>
-      <c r="J13" s="3">
-        <v>50</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>50</v>
+      </c>
+      <c r="K13">
         <v>0.2</v>
       </c>
       <c r="L13" s="2">
@@ -1530,55 +1530,760 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>365</v>
+      </c>
+      <c r="E14">
+        <v>128</v>
+      </c>
+      <c r="F14">
+        <v>600</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>150</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>50</v>
+      </c>
+      <c r="K14">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44802</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>365</v>
+      </c>
+      <c r="E15">
+        <v>512</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>200</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+      <c r="K15">
+        <v>0.2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44802</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>730</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>250</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44802</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>730</v>
+      </c>
+      <c r="E17">
         <v>7</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F17">
         <v>1000</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H17">
         <v>250</v>
       </c>
-      <c r="I14" s="2">
-        <v>100</v>
-      </c>
-      <c r="J14" s="2">
-        <v>50</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17">
         <v>0.2</v>
       </c>
-      <c r="L14" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="L17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>365</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>800</v>
+      </c>
+      <c r="G18" s="4">
+        <v>50</v>
+      </c>
+      <c r="H18" s="4">
+        <v>150</v>
+      </c>
+      <c r="I18" s="4">
+        <v>100</v>
+      </c>
+      <c r="J18" s="4">
+        <v>50</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>365</v>
+      </c>
+      <c r="E19" s="2">
+        <v>128</v>
+      </c>
+      <c r="F19" s="2">
+        <v>400</v>
+      </c>
+      <c r="G19" s="2">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2">
+        <v>150</v>
+      </c>
+      <c r="I19" s="2">
+        <v>100</v>
+      </c>
+      <c r="J19" s="2">
+        <v>50</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>365</v>
+      </c>
+      <c r="E20" s="4">
+        <v>128</v>
+      </c>
+      <c r="F20" s="4">
+        <v>600</v>
+      </c>
+      <c r="G20" s="4">
+        <v>50</v>
+      </c>
+      <c r="H20" s="4">
+        <v>150</v>
+      </c>
+      <c r="I20" s="4">
+        <v>100</v>
+      </c>
+      <c r="J20" s="4">
+        <v>50</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>365</v>
+      </c>
+      <c r="E21" s="2">
+        <v>512</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>50</v>
+      </c>
+      <c r="H21" s="2">
+        <v>200</v>
+      </c>
+      <c r="I21" s="2">
+        <v>100</v>
+      </c>
+      <c r="J21" s="2">
+        <v>50</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>365</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>600</v>
+      </c>
+      <c r="G22" s="4">
+        <v>50</v>
+      </c>
+      <c r="H22" s="4">
+        <v>150</v>
+      </c>
+      <c r="I22" s="4">
+        <v>100</v>
+      </c>
+      <c r="J22" s="4">
+        <v>50</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>365</v>
+      </c>
+      <c r="E23" s="4">
+        <v>128</v>
+      </c>
+      <c r="F23" s="4">
+        <v>600</v>
+      </c>
+      <c r="G23" s="4">
+        <v>50</v>
+      </c>
+      <c r="H23" s="4">
+        <v>150</v>
+      </c>
+      <c r="I23" s="4">
+        <v>100</v>
+      </c>
+      <c r="J23" s="4">
+        <v>50</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>730</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G24" s="2">
+        <v>40</v>
+      </c>
+      <c r="H24" s="2">
+        <v>250</v>
+      </c>
+      <c r="I24" s="2">
+        <v>100</v>
+      </c>
+      <c r="J24" s="2">
+        <v>50</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>365</v>
+      </c>
+      <c r="E25" s="2">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2">
+        <v>600</v>
+      </c>
+      <c r="G25" s="2">
+        <v>50</v>
+      </c>
+      <c r="H25" s="2">
+        <v>150</v>
+      </c>
+      <c r="I25" s="2">
+        <v>100</v>
+      </c>
+      <c r="J25" s="2">
+        <v>50</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>365</v>
+      </c>
+      <c r="E26" s="2">
+        <v>512</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="2">
+        <v>50</v>
+      </c>
+      <c r="H26" s="2">
+        <v>200</v>
+      </c>
+      <c r="I26" s="2">
+        <v>100</v>
+      </c>
+      <c r="J26" s="2">
+        <v>50</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>365</v>
+      </c>
+      <c r="E27" s="2">
+        <v>12</v>
+      </c>
+      <c r="F27" s="2">
+        <v>600</v>
+      </c>
+      <c r="G27" s="2">
+        <v>50</v>
+      </c>
+      <c r="H27" s="2">
+        <v>150</v>
+      </c>
+      <c r="I27" s="2">
+        <v>100</v>
+      </c>
+      <c r="J27" s="2">
+        <v>50</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>365</v>
+      </c>
+      <c r="E28" s="3">
+        <v>12</v>
+      </c>
+      <c r="F28" s="3">
+        <v>600</v>
+      </c>
+      <c r="G28" s="3">
+        <v>50</v>
+      </c>
+      <c r="H28" s="3">
+        <v>150</v>
+      </c>
+      <c r="I28" s="3">
+        <v>100</v>
+      </c>
+      <c r="J28" s="3">
+        <v>50</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>730</v>
+      </c>
+      <c r="E29" s="3">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G29" s="3">
+        <v>50</v>
+      </c>
+      <c r="H29" s="3">
+        <v>250</v>
+      </c>
+      <c r="I29" s="3">
+        <v>100</v>
+      </c>
+      <c r="J29" s="3">
+        <v>50</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44799</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>730</v>
+      </c>
+      <c r="E30" s="2">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G30" s="2">
+        <v>40</v>
+      </c>
+      <c r="H30" s="2">
+        <v>250</v>
+      </c>
+      <c r="I30" s="2">
+        <v>100</v>
+      </c>
+      <c r="J30" s="2">
+        <v>50</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N16">
-    <sortCondition ref="B2:B16"/>
-    <sortCondition ref="D2:D16"/>
-    <sortCondition ref="E2:E16"/>
-    <sortCondition ref="F2:F16"/>
-    <sortCondition ref="G2:G16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N32">
+    <sortCondition descending="1" ref="A2:A32"/>
+    <sortCondition ref="B2:B32"/>
+    <sortCondition ref="D2:D32"/>
+    <sortCondition ref="E2:E32"/>
+    <sortCondition ref="F2:F32"/>
+    <sortCondition ref="G2:G32"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>